<commit_message>
improve generate tables performance
</commit_message>
<xml_diff>
--- a/tests/VN8413_Data.xlsx
+++ b/tests/VN8413_Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/723e82af93afbbb8/Dev Area/PyPackages/packaging_dpkits/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="13_ncr:1_{7580FB57-E33F-4291-AE49-1D26396487B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9DF10CDE-CD9E-4F04-853E-E19A49418EE8}"/>
+  <xr:revisionPtr revIDLastSave="73" documentId="13_ncr:1_{7580FB57-E33F-4291-AE49-1D26396487B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BD6BCB17-FF5A-45B6-81F3-5057293F71E4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5093,22 +5093,22 @@
     <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6810,9 +6810,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:EF157"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DQ1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="BD1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="EF8" sqref="EF8"/>
+      <selection pane="bottomLeft" activeCell="BK5" sqref="BK5:BK7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6926,54 +6926,54 @@
       </c>
     </row>
     <row r="4" spans="1:136" x14ac:dyDescent="0.25">
-      <c r="BW4" s="32" t="s">
+      <c r="BW4" s="31" t="s">
         <v>160</v>
       </c>
-      <c r="BX4" s="32"/>
-      <c r="BY4" s="32"/>
-      <c r="BZ4" s="32"/>
-      <c r="CA4" s="32"/>
-      <c r="CB4" s="32"/>
-      <c r="CC4" s="32"/>
-      <c r="CD4" s="32"/>
-      <c r="CE4" s="32"/>
-      <c r="CF4" s="32"/>
-      <c r="CG4" s="32"/>
-      <c r="CH4" s="32"/>
-      <c r="CI4" s="32"/>
-      <c r="CJ4" s="32"/>
-      <c r="CK4" s="32" t="s">
+      <c r="BX4" s="31"/>
+      <c r="BY4" s="31"/>
+      <c r="BZ4" s="31"/>
+      <c r="CA4" s="31"/>
+      <c r="CB4" s="31"/>
+      <c r="CC4" s="31"/>
+      <c r="CD4" s="31"/>
+      <c r="CE4" s="31"/>
+      <c r="CF4" s="31"/>
+      <c r="CG4" s="31"/>
+      <c r="CH4" s="31"/>
+      <c r="CI4" s="31"/>
+      <c r="CJ4" s="31"/>
+      <c r="CK4" s="31" t="s">
         <v>161</v>
       </c>
-      <c r="CL4" s="32"/>
-      <c r="CM4" s="32"/>
-      <c r="CN4" s="32"/>
-      <c r="CO4" s="32"/>
-      <c r="CP4" s="32"/>
-      <c r="CQ4" s="32"/>
-      <c r="CR4" s="32"/>
-      <c r="CS4" s="32"/>
-      <c r="CT4" s="32"/>
-      <c r="CU4" s="32"/>
-      <c r="CV4" s="32"/>
-      <c r="CW4" s="32"/>
-      <c r="CX4" s="32"/>
-      <c r="CY4" s="32" t="s">
+      <c r="CL4" s="31"/>
+      <c r="CM4" s="31"/>
+      <c r="CN4" s="31"/>
+      <c r="CO4" s="31"/>
+      <c r="CP4" s="31"/>
+      <c r="CQ4" s="31"/>
+      <c r="CR4" s="31"/>
+      <c r="CS4" s="31"/>
+      <c r="CT4" s="31"/>
+      <c r="CU4" s="31"/>
+      <c r="CV4" s="31"/>
+      <c r="CW4" s="31"/>
+      <c r="CX4" s="31"/>
+      <c r="CY4" s="31" t="s">
         <v>162</v>
       </c>
-      <c r="CZ4" s="32"/>
-      <c r="DA4" s="32"/>
-      <c r="DB4" s="32"/>
-      <c r="DC4" s="32"/>
-      <c r="DD4" s="32"/>
-      <c r="DE4" s="32"/>
-      <c r="DF4" s="32"/>
-      <c r="DG4" s="32"/>
-      <c r="DH4" s="32"/>
-      <c r="DI4" s="32"/>
-      <c r="DJ4" s="32"/>
-      <c r="DK4" s="32"/>
-      <c r="DL4" s="32"/>
+      <c r="CZ4" s="31"/>
+      <c r="DA4" s="31"/>
+      <c r="DB4" s="31"/>
+      <c r="DC4" s="31"/>
+      <c r="DD4" s="31"/>
+      <c r="DE4" s="31"/>
+      <c r="DF4" s="31"/>
+      <c r="DG4" s="31"/>
+      <c r="DH4" s="31"/>
+      <c r="DI4" s="31"/>
+      <c r="DJ4" s="31"/>
+      <c r="DK4" s="31"/>
+      <c r="DL4" s="31"/>
     </row>
     <row r="5" spans="1:136" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="30" t="s">
@@ -7231,10 +7231,10 @@
       <c r="CK5" s="30" t="s">
         <v>130</v>
       </c>
-      <c r="CL5" s="31" t="s">
+      <c r="CL5" s="29" t="s">
         <v>131</v>
       </c>
-      <c r="CM5" s="31"/>
+      <c r="CM5" s="29"/>
       <c r="CN5" s="30" t="s">
         <v>132</v>
       </c>
@@ -7255,10 +7255,10 @@
         <v>138</v>
       </c>
       <c r="CU5" s="30"/>
-      <c r="CV5" s="31" t="s">
+      <c r="CV5" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="CW5" s="31"/>
+      <c r="CW5" s="29"/>
       <c r="CX5" s="30" t="s">
         <v>140</v>
       </c>
@@ -7269,10 +7269,10 @@
         <v>142</v>
       </c>
       <c r="DA5" s="30"/>
-      <c r="DB5" s="31" t="s">
+      <c r="DB5" s="29" t="s">
         <v>143</v>
       </c>
-      <c r="DC5" s="31"/>
+      <c r="DC5" s="29"/>
       <c r="DD5" s="30" t="s">
         <v>144</v>
       </c>
@@ -7289,20 +7289,20 @@
         <v>148</v>
       </c>
       <c r="DI5" s="30"/>
-      <c r="DJ5" s="31" t="s">
+      <c r="DJ5" s="29" t="s">
         <v>149</v>
       </c>
-      <c r="DK5" s="31"/>
+      <c r="DK5" s="29"/>
       <c r="DL5" s="30" t="s">
         <v>150</v>
       </c>
       <c r="DM5" s="30" t="s">
         <v>151</v>
       </c>
-      <c r="DN5" s="31" t="s">
+      <c r="DN5" s="29" t="s">
         <v>156</v>
       </c>
-      <c r="DO5" s="31"/>
+      <c r="DO5" s="29"/>
       <c r="DP5" s="30" t="s">
         <v>218</v>
       </c>
@@ -7311,43 +7311,43 @@
       </c>
       <c r="DR5" s="30"/>
       <c r="DS5" s="30"/>
-      <c r="DT5" s="31" t="s">
+      <c r="DT5" s="29" t="s">
         <v>540</v>
       </c>
-      <c r="DU5" s="33" t="s">
+      <c r="DU5" s="28" t="s">
         <v>549</v>
       </c>
-      <c r="DV5" s="33" t="s">
+      <c r="DV5" s="28" t="s">
         <v>550</v>
       </c>
-      <c r="DW5" s="33" t="s">
+      <c r="DW5" s="28" t="s">
         <v>551</v>
       </c>
-      <c r="DX5" s="33" t="s">
+      <c r="DX5" s="28" t="s">
         <v>552</v>
       </c>
-      <c r="DY5" s="33" t="s">
+      <c r="DY5" s="28" t="s">
         <v>553</v>
       </c>
-      <c r="DZ5" s="33" t="s">
+      <c r="DZ5" s="28" t="s">
         <v>554</v>
       </c>
-      <c r="EA5" s="29" t="s">
+      <c r="EA5" s="33" t="s">
         <v>1620</v>
       </c>
-      <c r="EB5" s="29" t="s">
+      <c r="EB5" s="33" t="s">
         <v>1621</v>
       </c>
-      <c r="EC5" s="29" t="s">
+      <c r="EC5" s="33" t="s">
         <v>1622</v>
       </c>
-      <c r="ED5" s="28" t="s">
+      <c r="ED5" s="32" t="s">
         <v>1623</v>
       </c>
-      <c r="EE5" s="28" t="s">
+      <c r="EE5" s="32" t="s">
         <v>1624</v>
       </c>
-      <c r="EF5" s="28" t="s">
+      <c r="EF5" s="32" t="s">
         <v>1625</v>
       </c>
     </row>
@@ -7441,8 +7441,8 @@
       <c r="CI6" s="30"/>
       <c r="CJ6" s="30"/>
       <c r="CK6" s="30"/>
-      <c r="CL6" s="31"/>
-      <c r="CM6" s="31"/>
+      <c r="CL6" s="29"/>
+      <c r="CM6" s="29"/>
       <c r="CN6" s="30"/>
       <c r="CO6" s="30"/>
       <c r="CP6" s="30"/>
@@ -7451,43 +7451,43 @@
       <c r="CS6" s="30"/>
       <c r="CT6" s="30"/>
       <c r="CU6" s="30"/>
-      <c r="CV6" s="31"/>
-      <c r="CW6" s="31"/>
+      <c r="CV6" s="29"/>
+      <c r="CW6" s="29"/>
       <c r="CX6" s="30"/>
       <c r="CY6" s="30"/>
       <c r="CZ6" s="30"/>
       <c r="DA6" s="30"/>
-      <c r="DB6" s="31"/>
-      <c r="DC6" s="31"/>
+      <c r="DB6" s="29"/>
+      <c r="DC6" s="29"/>
       <c r="DD6" s="30"/>
       <c r="DE6" s="30"/>
       <c r="DF6" s="30"/>
       <c r="DG6" s="30"/>
       <c r="DH6" s="30"/>
       <c r="DI6" s="30"/>
-      <c r="DJ6" s="31"/>
-      <c r="DK6" s="31"/>
+      <c r="DJ6" s="29"/>
+      <c r="DK6" s="29"/>
       <c r="DL6" s="30"/>
       <c r="DM6" s="30"/>
-      <c r="DN6" s="31"/>
-      <c r="DO6" s="31"/>
+      <c r="DN6" s="29"/>
+      <c r="DO6" s="29"/>
       <c r="DP6" s="30"/>
       <c r="DQ6" s="30"/>
       <c r="DR6" s="30"/>
       <c r="DS6" s="30"/>
-      <c r="DT6" s="31"/>
-      <c r="DU6" s="31"/>
-      <c r="DV6" s="31"/>
-      <c r="DW6" s="31"/>
-      <c r="DX6" s="31"/>
-      <c r="DY6" s="31"/>
-      <c r="DZ6" s="31"/>
-      <c r="EA6" s="29"/>
-      <c r="EB6" s="29"/>
-      <c r="EC6" s="29"/>
-      <c r="ED6" s="28"/>
-      <c r="EE6" s="28"/>
-      <c r="EF6" s="28"/>
+      <c r="DT6" s="29"/>
+      <c r="DU6" s="29"/>
+      <c r="DV6" s="29"/>
+      <c r="DW6" s="29"/>
+      <c r="DX6" s="29"/>
+      <c r="DY6" s="29"/>
+      <c r="DZ6" s="29"/>
+      <c r="EA6" s="33"/>
+      <c r="EB6" s="33"/>
+      <c r="EC6" s="33"/>
+      <c r="ED6" s="32"/>
+      <c r="EE6" s="32"/>
+      <c r="EF6" s="32"/>
     </row>
     <row r="7" spans="1:136" s="13" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="30"/>
@@ -7681,19 +7681,19 @@
       <c r="DS7" s="11" t="s">
         <v>224</v>
       </c>
-      <c r="DT7" s="31"/>
-      <c r="DU7" s="31"/>
-      <c r="DV7" s="31"/>
-      <c r="DW7" s="31"/>
-      <c r="DX7" s="31"/>
-      <c r="DY7" s="31"/>
-      <c r="DZ7" s="31"/>
-      <c r="EA7" s="29"/>
-      <c r="EB7" s="29"/>
-      <c r="EC7" s="29"/>
-      <c r="ED7" s="28"/>
-      <c r="EE7" s="28"/>
-      <c r="EF7" s="28"/>
+      <c r="DT7" s="29"/>
+      <c r="DU7" s="29"/>
+      <c r="DV7" s="29"/>
+      <c r="DW7" s="29"/>
+      <c r="DX7" s="29"/>
+      <c r="DY7" s="29"/>
+      <c r="DZ7" s="29"/>
+      <c r="EA7" s="33"/>
+      <c r="EB7" s="33"/>
+      <c r="EC7" s="33"/>
+      <c r="ED7" s="32"/>
+      <c r="EE7" s="32"/>
+      <c r="EF7" s="32"/>
     </row>
     <row r="8" spans="1:136" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
@@ -7774,9 +7774,7 @@
       <c r="BL8" s="19">
         <v>3</v>
       </c>
-      <c r="BM8" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM8" s="22"/>
       <c r="BN8" s="19">
         <v>1</v>
       </c>
@@ -8033,9 +8031,7 @@
       <c r="BL9" s="19">
         <v>3</v>
       </c>
-      <c r="BM9" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM9" s="22"/>
       <c r="BN9" s="19">
         <v>1</v>
       </c>
@@ -8296,9 +8292,7 @@
       <c r="BL10" s="19">
         <v>1</v>
       </c>
-      <c r="BM10" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM10" s="22"/>
       <c r="BN10" s="19">
         <v>1</v>
       </c>
@@ -9079,9 +9073,7 @@
       <c r="BL13" s="19">
         <v>3</v>
       </c>
-      <c r="BM13" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM13" s="22"/>
       <c r="BN13" s="19">
         <v>1</v>
       </c>
@@ -9593,9 +9585,7 @@
       <c r="BL15" s="19">
         <v>2</v>
       </c>
-      <c r="BM15" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM15" s="22"/>
       <c r="BN15" s="19">
         <v>1</v>
       </c>
@@ -9854,9 +9844,7 @@
       <c r="BL16" s="19">
         <v>3</v>
       </c>
-      <c r="BM16" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM16" s="22"/>
       <c r="BN16" s="19">
         <v>1</v>
       </c>
@@ -10117,9 +10105,7 @@
       <c r="BL17" s="19">
         <v>1</v>
       </c>
-      <c r="BM17" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM17" s="22"/>
       <c r="BN17" s="19">
         <v>1</v>
       </c>
@@ -10374,9 +10360,7 @@
       <c r="BL18" s="19">
         <v>2</v>
       </c>
-      <c r="BM18" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM18" s="22"/>
       <c r="BN18" s="19">
         <v>1</v>
       </c>
@@ -10629,9 +10613,7 @@
       <c r="BL19" s="19">
         <v>1</v>
       </c>
-      <c r="BM19" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM19" s="22"/>
       <c r="BN19" s="19">
         <v>1</v>
       </c>
@@ -10890,9 +10872,7 @@
       <c r="BL20" s="19">
         <v>3</v>
       </c>
-      <c r="BM20" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM20" s="22"/>
       <c r="BN20" s="19">
         <v>1</v>
       </c>
@@ -11145,9 +11125,7 @@
       <c r="BL21" s="19">
         <v>1</v>
       </c>
-      <c r="BM21" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM21" s="22"/>
       <c r="BN21" s="19">
         <v>1</v>
       </c>
@@ -11406,9 +11384,7 @@
       <c r="BL22" s="19">
         <v>3</v>
       </c>
-      <c r="BM22" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM22" s="22"/>
       <c r="BN22" s="19">
         <v>1</v>
       </c>
@@ -11669,9 +11645,7 @@
       <c r="BL23" s="19">
         <v>3</v>
       </c>
-      <c r="BM23" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM23" s="22"/>
       <c r="BN23" s="19">
         <v>1</v>
       </c>
@@ -11932,9 +11906,7 @@
       <c r="BL24" s="19">
         <v>2</v>
       </c>
-      <c r="BM24" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM24" s="22"/>
       <c r="BN24" s="19">
         <v>1</v>
       </c>
@@ -12189,9 +12161,7 @@
       <c r="BL25" s="19">
         <v>3</v>
       </c>
-      <c r="BM25" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM25" s="22"/>
       <c r="BN25" s="19">
         <v>1</v>
       </c>
@@ -12448,9 +12418,7 @@
       <c r="BL26" s="19">
         <v>3</v>
       </c>
-      <c r="BM26" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM26" s="22"/>
       <c r="BN26" s="19">
         <v>1</v>
       </c>
@@ -12705,9 +12673,7 @@
       <c r="BL27" s="19">
         <v>1</v>
       </c>
-      <c r="BM27" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM27" s="22"/>
       <c r="BN27" s="19">
         <v>1</v>
       </c>
@@ -13231,9 +13197,7 @@
       <c r="BL29" s="19">
         <v>3</v>
       </c>
-      <c r="BM29" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM29" s="22"/>
       <c r="BN29" s="19">
         <v>1</v>
       </c>
@@ -13492,9 +13456,7 @@
       <c r="BL30" s="19">
         <v>1</v>
       </c>
-      <c r="BM30" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM30" s="22"/>
       <c r="BN30" s="19">
         <v>1</v>
       </c>
@@ -13751,9 +13713,7 @@
       <c r="BL31" s="19">
         <v>2</v>
       </c>
-      <c r="BM31" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM31" s="22"/>
       <c r="BN31" s="19">
         <v>1</v>
       </c>
@@ -14014,9 +13974,7 @@
       <c r="BL32" s="19">
         <v>2</v>
       </c>
-      <c r="BM32" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM32" s="22"/>
       <c r="BN32" s="19">
         <v>1</v>
       </c>
@@ -14795,9 +14753,7 @@
       <c r="BL35" s="19">
         <v>2</v>
       </c>
-      <c r="BM35" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM35" s="22"/>
       <c r="BN35" s="19">
         <v>1</v>
       </c>
@@ -15058,9 +15014,7 @@
       <c r="BL36" s="19">
         <v>2</v>
       </c>
-      <c r="BM36" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM36" s="22"/>
       <c r="BN36" s="19">
         <v>1</v>
       </c>
@@ -15321,9 +15275,7 @@
       <c r="BL37" s="19">
         <v>3</v>
       </c>
-      <c r="BM37" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM37" s="22"/>
       <c r="BN37" s="19">
         <v>1</v>
       </c>
@@ -15841,9 +15793,7 @@
       <c r="BL39" s="19">
         <v>3</v>
       </c>
-      <c r="BM39" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM39" s="22"/>
       <c r="BN39" s="19">
         <v>1</v>
       </c>
@@ -16104,9 +16054,7 @@
       <c r="BL40" s="19">
         <v>1</v>
       </c>
-      <c r="BM40" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM40" s="22"/>
       <c r="BN40" s="19">
         <v>1</v>
       </c>
@@ -16365,9 +16313,7 @@
       <c r="BL41" s="19">
         <v>2</v>
       </c>
-      <c r="BM41" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM41" s="22"/>
       <c r="BN41" s="19">
         <v>1</v>
       </c>
@@ -16628,9 +16574,7 @@
       <c r="BL42" s="19">
         <v>3</v>
       </c>
-      <c r="BM42" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM42" s="22"/>
       <c r="BN42" s="19">
         <v>1</v>
       </c>
@@ -16891,9 +16835,7 @@
       <c r="BL43" s="19">
         <v>1</v>
       </c>
-      <c r="BM43" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM43" s="22"/>
       <c r="BN43" s="19">
         <v>1</v>
       </c>
@@ -17150,9 +17092,7 @@
       <c r="BL44" s="19">
         <v>2</v>
       </c>
-      <c r="BM44" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM44" s="22"/>
       <c r="BN44" s="19">
         <v>1</v>
       </c>
@@ -17413,9 +17353,7 @@
       <c r="BL45" s="19">
         <v>2</v>
       </c>
-      <c r="BM45" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM45" s="22"/>
       <c r="BN45" s="19">
         <v>1</v>
       </c>
@@ -17674,9 +17612,7 @@
       <c r="BL46" s="19">
         <v>3</v>
       </c>
-      <c r="BM46" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM46" s="22"/>
       <c r="BN46" s="19">
         <v>1</v>
       </c>
@@ -17931,9 +17867,7 @@
       <c r="BL47" s="19">
         <v>2</v>
       </c>
-      <c r="BM47" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM47" s="22"/>
       <c r="BN47" s="19">
         <v>1</v>
       </c>
@@ -18190,9 +18124,7 @@
       <c r="BL48" s="19">
         <v>2</v>
       </c>
-      <c r="BM48" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM48" s="22"/>
       <c r="BN48" s="19">
         <v>1</v>
       </c>
@@ -18451,9 +18383,7 @@
       <c r="BL49" s="19">
         <v>1</v>
       </c>
-      <c r="BM49" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM49" s="22"/>
       <c r="BN49" s="19">
         <v>1</v>
       </c>
@@ -18710,9 +18640,7 @@
       <c r="BL50" s="19">
         <v>3</v>
       </c>
-      <c r="BM50" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM50" s="22"/>
       <c r="BN50" s="19">
         <v>1</v>
       </c>
@@ -18973,9 +18901,7 @@
       <c r="BL51" s="19">
         <v>2</v>
       </c>
-      <c r="BM51" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM51" s="22"/>
       <c r="BN51" s="19">
         <v>1</v>
       </c>
@@ -19232,9 +19158,7 @@
       <c r="BL52" s="19">
         <v>2</v>
       </c>
-      <c r="BM52" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM52" s="22"/>
       <c r="BN52" s="19">
         <v>1</v>
       </c>
@@ -19495,9 +19419,7 @@
       <c r="BL53" s="19">
         <v>3</v>
       </c>
-      <c r="BM53" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM53" s="22"/>
       <c r="BN53" s="19">
         <v>1</v>
       </c>
@@ -19758,9 +19680,7 @@
       <c r="BL54" s="19">
         <v>3</v>
       </c>
-      <c r="BM54" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM54" s="22"/>
       <c r="BN54" s="19">
         <v>1</v>
       </c>
@@ -20019,9 +19939,7 @@
       <c r="BL55" s="19">
         <v>1</v>
       </c>
-      <c r="BM55" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM55" s="22"/>
       <c r="BN55" s="19">
         <v>1</v>
       </c>
@@ -20282,9 +20200,7 @@
       <c r="BL56" s="19">
         <v>1</v>
       </c>
-      <c r="BM56" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM56" s="22"/>
       <c r="BN56" s="19">
         <v>1</v>
       </c>
@@ -20543,9 +20459,7 @@
       <c r="BL57" s="19">
         <v>3</v>
       </c>
-      <c r="BM57" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM57" s="22"/>
       <c r="BN57" s="19">
         <v>1</v>
       </c>
@@ -20806,9 +20720,7 @@
       <c r="BL58" s="19">
         <v>2</v>
       </c>
-      <c r="BM58" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM58" s="22"/>
       <c r="BN58" s="19">
         <v>1</v>
       </c>
@@ -21069,9 +20981,7 @@
       <c r="BL59" s="19">
         <v>3</v>
       </c>
-      <c r="BM59" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM59" s="22"/>
       <c r="BN59" s="19">
         <v>1</v>
       </c>
@@ -21332,9 +21242,7 @@
       <c r="BL60" s="19">
         <v>2</v>
       </c>
-      <c r="BM60" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM60" s="22"/>
       <c r="BN60" s="19">
         <v>1</v>
       </c>
@@ -21593,9 +21501,7 @@
       <c r="BL61" s="19">
         <v>3</v>
       </c>
-      <c r="BM61" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM61" s="22"/>
       <c r="BN61" s="19">
         <v>1</v>
       </c>
@@ -21856,9 +21762,7 @@
       <c r="BL62" s="19">
         <v>1</v>
       </c>
-      <c r="BM62" s="19">
-        <v>2</v>
-      </c>
+      <c r="BM62" s="22"/>
       <c r="BN62" s="19">
         <v>1</v>
       </c>
@@ -22119,9 +22023,7 @@
       <c r="BL63" s="3">
         <v>3</v>
       </c>
-      <c r="BM63" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM63" s="23"/>
       <c r="BN63" s="3">
         <v>1</v>
       </c>
@@ -22380,9 +22282,7 @@
       <c r="BL64" s="3">
         <v>2</v>
       </c>
-      <c r="BM64" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM64" s="23"/>
       <c r="BN64" s="3">
         <v>1</v>
       </c>
@@ -22643,9 +22543,7 @@
       <c r="BL65" s="3">
         <v>2</v>
       </c>
-      <c r="BM65" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM65" s="23"/>
       <c r="BN65" s="3">
         <v>1</v>
       </c>
@@ -22906,9 +22804,7 @@
       <c r="BL66" s="3">
         <v>3</v>
       </c>
-      <c r="BM66" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM66" s="23"/>
       <c r="BN66" s="3">
         <v>1</v>
       </c>
@@ -23169,9 +23065,7 @@
       <c r="BL67" s="3">
         <v>3</v>
       </c>
-      <c r="BM67" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM67" s="23"/>
       <c r="BN67" s="3">
         <v>1</v>
       </c>
@@ -23689,9 +23583,7 @@
       <c r="BL69" s="3">
         <v>2</v>
       </c>
-      <c r="BM69" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM69" s="23"/>
       <c r="BN69" s="3">
         <v>1</v>
       </c>
@@ -23946,9 +23838,7 @@
       <c r="BL70" s="3">
         <v>1</v>
       </c>
-      <c r="BM70" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM70" s="23"/>
       <c r="BN70" s="3">
         <v>1</v>
       </c>
@@ -24466,9 +24356,7 @@
       <c r="BL72" s="3">
         <v>3</v>
       </c>
-      <c r="BM72" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM72" s="23"/>
       <c r="BN72" s="3">
         <v>1</v>
       </c>
@@ -24727,9 +24615,7 @@
       <c r="BL73" s="3">
         <v>1</v>
       </c>
-      <c r="BM73" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM73" s="23"/>
       <c r="BN73" s="3">
         <v>1</v>
       </c>
@@ -24990,9 +24876,7 @@
       <c r="BL74" s="3">
         <v>3</v>
       </c>
-      <c r="BM74" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM74" s="23"/>
       <c r="BN74" s="3">
         <v>1</v>
       </c>
@@ -25245,9 +25129,7 @@
       <c r="BL75" s="3">
         <v>3</v>
       </c>
-      <c r="BM75" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM75" s="23"/>
       <c r="BN75" s="3">
         <v>1</v>
       </c>
@@ -25767,9 +25649,7 @@
       <c r="BL77" s="3">
         <v>1</v>
       </c>
-      <c r="BM77" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM77" s="23"/>
       <c r="BN77" s="3">
         <v>1</v>
       </c>
@@ -26030,9 +25910,7 @@
       <c r="BL78" s="3">
         <v>1</v>
       </c>
-      <c r="BM78" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM78" s="23"/>
       <c r="BN78" s="3">
         <v>1</v>
       </c>
@@ -26293,9 +26171,7 @@
       <c r="BL79" s="3">
         <v>3</v>
       </c>
-      <c r="BM79" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM79" s="23"/>
       <c r="BN79" s="3">
         <v>1</v>
       </c>
@@ -26817,9 +26693,7 @@
       <c r="BL81" s="3">
         <v>1</v>
       </c>
-      <c r="BM81" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM81" s="23"/>
       <c r="BN81" s="3">
         <v>1</v>
       </c>
@@ -27857,9 +27731,7 @@
       <c r="BL85" s="3">
         <v>2</v>
       </c>
-      <c r="BM85" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM85" s="23"/>
       <c r="BN85" s="3">
         <v>1</v>
       </c>
@@ -28116,9 +27988,7 @@
       <c r="BL86" s="3">
         <v>2</v>
       </c>
-      <c r="BM86" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM86" s="23"/>
       <c r="BN86" s="3">
         <v>1</v>
       </c>
@@ -28379,9 +28249,7 @@
       <c r="BL87" s="3">
         <v>3</v>
       </c>
-      <c r="BM87" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM87" s="23"/>
       <c r="BN87" s="3">
         <v>1</v>
       </c>
@@ -28893,9 +28761,7 @@
       <c r="BL89" s="3">
         <v>2</v>
       </c>
-      <c r="BM89" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM89" s="23"/>
       <c r="BN89" s="3">
         <v>1</v>
       </c>
@@ -29674,9 +29540,7 @@
       <c r="BL92" s="3">
         <v>2</v>
       </c>
-      <c r="BM92" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM92" s="23"/>
       <c r="BN92" s="3">
         <v>1</v>
       </c>
@@ -30453,9 +30317,7 @@
       <c r="BL95" s="3">
         <v>2</v>
       </c>
-      <c r="BM95" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM95" s="23"/>
       <c r="BN95" s="3">
         <v>1</v>
       </c>
@@ -30971,9 +30833,7 @@
       <c r="BL97" s="3">
         <v>3</v>
       </c>
-      <c r="BM97" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM97" s="23"/>
       <c r="BN97" s="3">
         <v>1</v>
       </c>
@@ -37436,9 +37296,7 @@
       <c r="BL122" s="3">
         <v>2</v>
       </c>
-      <c r="BM122" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM122" s="23"/>
       <c r="BN122" s="3">
         <v>1</v>
       </c>
@@ -37954,9 +37812,7 @@
       <c r="BL124" s="3">
         <v>3</v>
       </c>
-      <c r="BM124" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM124" s="23"/>
       <c r="BN124" s="3">
         <v>1</v>
       </c>
@@ -41068,9 +40924,7 @@
       <c r="BL136" s="3">
         <v>1</v>
       </c>
-      <c r="BM136" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM136" s="23"/>
       <c r="BN136" s="3">
         <v>1</v>
       </c>
@@ -42881,9 +42735,7 @@
       <c r="BL143" s="3">
         <v>1</v>
       </c>
-      <c r="BM143" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM143" s="23"/>
       <c r="BN143" s="3">
         <v>1</v>
       </c>
@@ -43909,9 +43761,7 @@
       <c r="BL147" s="3">
         <v>2</v>
       </c>
-      <c r="BM147" s="3">
-        <v>2</v>
-      </c>
+      <c r="BM147" s="23"/>
       <c r="BN147" s="3">
         <v>1</v>
       </c>
@@ -46373,15 +46223,95 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <autoFilter ref="A7:EF157" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
   <mergeCells count="122">
-    <mergeCell ref="DW5:DW7"/>
-    <mergeCell ref="DX5:DX7"/>
-    <mergeCell ref="DY5:DY7"/>
-    <mergeCell ref="DZ5:DZ7"/>
-    <mergeCell ref="DP5:DP6"/>
-    <mergeCell ref="DQ5:DS6"/>
-    <mergeCell ref="DT5:DT7"/>
-    <mergeCell ref="DU5:DU7"/>
-    <mergeCell ref="DV5:DV7"/>
+    <mergeCell ref="EF5:EF7"/>
+    <mergeCell ref="EA5:EA7"/>
+    <mergeCell ref="EB5:EB7"/>
+    <mergeCell ref="EC5:EC7"/>
+    <mergeCell ref="ED5:ED7"/>
+    <mergeCell ref="EE5:EE7"/>
+    <mergeCell ref="F5:F7"/>
+    <mergeCell ref="G5:G7"/>
+    <mergeCell ref="H5:H7"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="J5:J7"/>
+    <mergeCell ref="T5:T7"/>
+    <mergeCell ref="Z5:Z7"/>
+    <mergeCell ref="AA5:AA7"/>
+    <mergeCell ref="AB5:AB7"/>
+    <mergeCell ref="AC5:AC7"/>
+    <mergeCell ref="AD5:AD7"/>
+    <mergeCell ref="U5:U7"/>
+    <mergeCell ref="V5:V7"/>
+    <mergeCell ref="W5:W7"/>
+    <mergeCell ref="X5:X7"/>
+    <mergeCell ref="Y5:Y7"/>
+    <mergeCell ref="AJ5:AJ7"/>
+    <mergeCell ref="AK5:AK7"/>
+    <mergeCell ref="A5:A7"/>
+    <mergeCell ref="B5:B7"/>
+    <mergeCell ref="C5:C7"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="E5:E7"/>
+    <mergeCell ref="P5:P7"/>
+    <mergeCell ref="Q5:Q7"/>
+    <mergeCell ref="R5:R7"/>
+    <mergeCell ref="S5:S7"/>
+    <mergeCell ref="K5:K7"/>
+    <mergeCell ref="L5:L7"/>
+    <mergeCell ref="M5:M7"/>
+    <mergeCell ref="N5:N7"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="AL5:AL7"/>
+    <mergeCell ref="AM5:AM7"/>
+    <mergeCell ref="AN5:AN7"/>
+    <mergeCell ref="AE5:AE7"/>
+    <mergeCell ref="AF5:AF7"/>
+    <mergeCell ref="AG5:AG7"/>
+    <mergeCell ref="AH5:AH7"/>
+    <mergeCell ref="AI5:AI7"/>
+    <mergeCell ref="AT5:AT7"/>
+    <mergeCell ref="AU5:AU7"/>
+    <mergeCell ref="AV5:AV7"/>
+    <mergeCell ref="AW5:AW7"/>
+    <mergeCell ref="AX5:AX7"/>
+    <mergeCell ref="AO5:AO7"/>
+    <mergeCell ref="AP5:AP7"/>
+    <mergeCell ref="AQ5:AQ7"/>
+    <mergeCell ref="AR5:AR7"/>
+    <mergeCell ref="AS5:AS7"/>
+    <mergeCell ref="BD5:BE6"/>
+    <mergeCell ref="BF5:BG6"/>
+    <mergeCell ref="BH5:BH7"/>
+    <mergeCell ref="BI5:BI7"/>
+    <mergeCell ref="BJ5:BJ7"/>
+    <mergeCell ref="AY5:AY7"/>
+    <mergeCell ref="AZ5:AZ7"/>
+    <mergeCell ref="BA5:BA7"/>
+    <mergeCell ref="BB5:BB7"/>
+    <mergeCell ref="BC5:BC7"/>
+    <mergeCell ref="BP5:BP7"/>
+    <mergeCell ref="BQ5:BQ7"/>
+    <mergeCell ref="BR5:BR7"/>
+    <mergeCell ref="BS5:BS7"/>
+    <mergeCell ref="BT5:BT7"/>
+    <mergeCell ref="BK5:BK7"/>
+    <mergeCell ref="BL5:BL7"/>
+    <mergeCell ref="BM5:BM7"/>
+    <mergeCell ref="BN5:BN7"/>
+    <mergeCell ref="BO5:BO7"/>
+    <mergeCell ref="CK5:CK7"/>
+    <mergeCell ref="CL5:CM6"/>
+    <mergeCell ref="CN5:CO6"/>
+    <mergeCell ref="CB5:CB7"/>
+    <mergeCell ref="CC5:CC7"/>
+    <mergeCell ref="CD5:CD7"/>
+    <mergeCell ref="CE5:CE7"/>
+    <mergeCell ref="CF5:CG6"/>
+    <mergeCell ref="BU5:BU7"/>
+    <mergeCell ref="BV5:BV7"/>
+    <mergeCell ref="BW5:BW7"/>
+    <mergeCell ref="BX5:BY6"/>
+    <mergeCell ref="BZ5:CA6"/>
     <mergeCell ref="DJ5:DK6"/>
     <mergeCell ref="DL5:DL7"/>
     <mergeCell ref="DM5:DM7"/>
@@ -46406,95 +46336,15 @@
     <mergeCell ref="CT5:CU6"/>
     <mergeCell ref="CH5:CI6"/>
     <mergeCell ref="CJ5:CJ7"/>
-    <mergeCell ref="CK5:CK7"/>
-    <mergeCell ref="CL5:CM6"/>
-    <mergeCell ref="CN5:CO6"/>
-    <mergeCell ref="CB5:CB7"/>
-    <mergeCell ref="CC5:CC7"/>
-    <mergeCell ref="CD5:CD7"/>
-    <mergeCell ref="CE5:CE7"/>
-    <mergeCell ref="CF5:CG6"/>
-    <mergeCell ref="BU5:BU7"/>
-    <mergeCell ref="BV5:BV7"/>
-    <mergeCell ref="BW5:BW7"/>
-    <mergeCell ref="BX5:BY6"/>
-    <mergeCell ref="BZ5:CA6"/>
-    <mergeCell ref="BP5:BP7"/>
-    <mergeCell ref="BQ5:BQ7"/>
-    <mergeCell ref="BR5:BR7"/>
-    <mergeCell ref="BS5:BS7"/>
-    <mergeCell ref="BT5:BT7"/>
-    <mergeCell ref="BK5:BK7"/>
-    <mergeCell ref="BL5:BL7"/>
-    <mergeCell ref="BM5:BM7"/>
-    <mergeCell ref="BN5:BN7"/>
-    <mergeCell ref="BO5:BO7"/>
-    <mergeCell ref="BD5:BE6"/>
-    <mergeCell ref="BF5:BG6"/>
-    <mergeCell ref="BH5:BH7"/>
-    <mergeCell ref="BI5:BI7"/>
-    <mergeCell ref="BJ5:BJ7"/>
-    <mergeCell ref="AY5:AY7"/>
-    <mergeCell ref="AZ5:AZ7"/>
-    <mergeCell ref="BA5:BA7"/>
-    <mergeCell ref="BB5:BB7"/>
-    <mergeCell ref="BC5:BC7"/>
-    <mergeCell ref="AU5:AU7"/>
-    <mergeCell ref="AV5:AV7"/>
-    <mergeCell ref="AW5:AW7"/>
-    <mergeCell ref="AX5:AX7"/>
-    <mergeCell ref="AO5:AO7"/>
-    <mergeCell ref="AP5:AP7"/>
-    <mergeCell ref="AQ5:AQ7"/>
-    <mergeCell ref="AR5:AR7"/>
-    <mergeCell ref="AS5:AS7"/>
-    <mergeCell ref="AL5:AL7"/>
-    <mergeCell ref="AM5:AM7"/>
-    <mergeCell ref="AN5:AN7"/>
-    <mergeCell ref="AE5:AE7"/>
-    <mergeCell ref="AF5:AF7"/>
-    <mergeCell ref="AG5:AG7"/>
-    <mergeCell ref="AH5:AH7"/>
-    <mergeCell ref="AI5:AI7"/>
-    <mergeCell ref="AT5:AT7"/>
-    <mergeCell ref="A5:A7"/>
-    <mergeCell ref="B5:B7"/>
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="E5:E7"/>
-    <mergeCell ref="P5:P7"/>
-    <mergeCell ref="Q5:Q7"/>
-    <mergeCell ref="R5:R7"/>
-    <mergeCell ref="S5:S7"/>
-    <mergeCell ref="K5:K7"/>
-    <mergeCell ref="L5:L7"/>
-    <mergeCell ref="M5:M7"/>
-    <mergeCell ref="N5:N7"/>
-    <mergeCell ref="O5:O7"/>
-    <mergeCell ref="EF5:EF7"/>
-    <mergeCell ref="EA5:EA7"/>
-    <mergeCell ref="EB5:EB7"/>
-    <mergeCell ref="EC5:EC7"/>
-    <mergeCell ref="ED5:ED7"/>
-    <mergeCell ref="EE5:EE7"/>
-    <mergeCell ref="F5:F7"/>
-    <mergeCell ref="G5:G7"/>
-    <mergeCell ref="H5:H7"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="J5:J7"/>
-    <mergeCell ref="T5:T7"/>
-    <mergeCell ref="Z5:Z7"/>
-    <mergeCell ref="AA5:AA7"/>
-    <mergeCell ref="AB5:AB7"/>
-    <mergeCell ref="AC5:AC7"/>
-    <mergeCell ref="AD5:AD7"/>
-    <mergeCell ref="U5:U7"/>
-    <mergeCell ref="V5:V7"/>
-    <mergeCell ref="W5:W7"/>
-    <mergeCell ref="X5:X7"/>
-    <mergeCell ref="Y5:Y7"/>
-    <mergeCell ref="AJ5:AJ7"/>
-    <mergeCell ref="AK5:AK7"/>
+    <mergeCell ref="DW5:DW7"/>
+    <mergeCell ref="DX5:DX7"/>
+    <mergeCell ref="DY5:DY7"/>
+    <mergeCell ref="DZ5:DZ7"/>
+    <mergeCell ref="DP5:DP6"/>
+    <mergeCell ref="DQ5:DS6"/>
+    <mergeCell ref="DT5:DT7"/>
+    <mergeCell ref="DU5:DU7"/>
+    <mergeCell ref="DV5:DV7"/>
   </mergeCells>
   <conditionalFormatting sqref="DN8:DN157">
     <cfRule type="duplicateValues" dxfId="1" priority="5"/>

</xml_diff>